<commit_message>
signin modified a little
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTestData/testdata1.xlsx
+++ b/src/test/resources/excelTestData/testdata1.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="login-valid" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="login-invalid" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="login_valid" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="login_invalid" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Scenarioname</t>
   </si>
@@ -44,6 +44,12 @@
     <t>automation2025#</t>
   </si>
   <si>
+    <t>ScenarioName</t>
+  </si>
+  <si>
+    <t>expectedErrMsg</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
@@ -63,12 +69,6 @@
   </si>
   <si>
     <t>Empty username and valid password</t>
-  </si>
-  <si>
-    <t>Sweet@123</t>
-  </si>
-  <si>
-    <t>cvbnm1234</t>
   </si>
   <si>
     <t>Invalid username and valid password</t>
@@ -90,7 +90,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -107,13 +107,8 @@
       <color rgb="FF000000"/>
       <name val="&quot;Consolas&quot;"/>
     </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF008000"/>
-      <name val="&quot;Consolas&quot;"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,12 +121,6 @@
         <bgColor rgb="FFD4D4D4"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -139,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -150,12 +139,6 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -446,114 +429,86 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>